<commit_message>
Add the leave account function
</commit_message>
<xml_diff>
--- a/server/docs/노크 데이터베이스 정의서 초안_서버_v3.6.xlsx
+++ b/server/docs/노크 데이터베이스 정의서 초안_서버_v3.6.xlsx
@@ -5110,10 +5110,10 @@
   <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -5318,7 +5318,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>265</v>
+        <v>85</v>
       </c>
       <c r="D10" s="41">
         <v>45</v>
@@ -5418,7 +5418,7 @@
         <v>185</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>265</v>
+        <v>87</v>
       </c>
       <c r="D15" s="41">
         <v>45</v>
@@ -5438,7 +5438,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D16" s="41">
         <v>45</v>
@@ -6133,7 +6133,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>